<commit_message>
Se quitan signos de admiracion en los alerts de preguntas
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -5,18 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A66204E-2EEF-40BA-A2C1-8888C483A810}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83F7ACC-0183-41F4-ADA3-583CAF2FB935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -197,7 +196,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,36 +228,45 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,249 +584,249 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:L3"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
       <c r="M3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
       <c r="M4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
       <c r="M5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
       <c r="M6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
       <c r="M8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
       <c r="M10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
       <c r="M11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
       <c r="M12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
       <c r="M13" t="s">
         <v>33</v>
       </c>
@@ -837,20 +851,20 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="1" t="s">
         <v>33</v>
       </c>
@@ -875,58 +889,58 @@
       </c>
     </row>
     <row r="17" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
       <c r="M17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
       <c r="M18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
       <c r="M19" t="s">
         <v>34</v>
       </c>
@@ -951,134 +965,134 @@
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
       <c r="M21" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
       <c r="M22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
       <c r="M23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
       <c r="M24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
       <c r="M25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1142,20 +1156,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A21:L21"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="A17:L17"/>
@@ -1169,6 +1169,20 @@
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
se actualizan actividades del excel
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C83F7ACC-0183-41F4-ADA3-583CAF2FB935}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9A75FE-F682-4D3D-A977-D775C054336E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
@@ -228,23 +228,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -253,20 +262,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,192 +581,192 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:L22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
       <c r="M3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
       <c r="M5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
       <c r="M6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
       <c r="M7" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
       <c r="M10" t="s">
         <v>33</v>
       </c>
@@ -794,134 +791,134 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
       <c r="M12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
       <c r="M13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
       <c r="M14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
       <c r="M16" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
-      <c r="L17" s="3"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
       <c r="M18" t="s">
         <v>34</v>
       </c>
@@ -946,20 +943,20 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
       <c r="M20" t="s">
         <v>33</v>
       </c>
@@ -984,115 +981,115 @@
       </c>
     </row>
     <row r="22" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
       <c r="M22" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
       <c r="M23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
       <c r="M24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
       <c r="M25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
+      <c r="B26" s="10"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
       <c r="M26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
       <c r="M27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1156,19 +1153,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A10:L10"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A25:L25"/>
@@ -1183,6 +1167,19 @@
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A15:L15"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agrega columna de precio en el reporte de compras, se agrega columna de costo en productos, se agrega columna de costo en el reporte de inventario y se corrigen errores de visualizacion en los reportes
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\comer\Analisis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yessy\Desktop\PROYECTO\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9A75FE-F682-4D3D-A977-D775C054336E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA439DAF-827E-4CC1-8D60-81C11ADB7F37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
@@ -228,31 +228,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -262,8 +241,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,59 +584,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
   <dimension ref="A1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:L17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
       <c r="M3" t="s">
         <v>34</v>
       </c>
@@ -658,58 +661,58 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
       <c r="M6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
       <c r="M7" t="s">
         <v>34</v>
       </c>
@@ -753,96 +756,96 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
       <c r="M10" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
       <c r="M11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
       <c r="M12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
       <c r="M13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" t="s">
         <v>37</v>
       </c>
@@ -867,20 +870,20 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
       <c r="M16" t="s">
         <v>34</v>
       </c>
@@ -905,77 +908,77 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
       <c r="M19" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
+      <c r="B20" s="9"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
       <c r="M20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
       <c r="M21" t="s">
         <v>34</v>
       </c>
@@ -1000,96 +1003,96 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
       <c r="M23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
       <c r="M24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="M25" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="M26" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
       <c r="M27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1153,6 +1156,19 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A10:L10"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A25:L25"/>
@@ -1167,19 +1183,6 @@
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
1.-permisos quedan a nivel de inicio de sesion falta validar a nivel de url en navegador 2.-se agrega al login  el loader al mandar a validar 3.- se hacen algunas actividades del excel
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9A0328-2774-4AD9-AF52-9FB936EF4F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1580F-EBF8-4669-83EF-4B393BE1FF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>- Agregar precio de menudeo y mayoreo en la información de los productos en venta con una abreviatura que identifique el precio p.e. “Me:” o “Ma:”. Además, cambiar existencias a abreviado “E: ” y si no hay poner “S/E”.</t>
   </si>
@@ -166,13 +166,28 @@
   </si>
   <si>
     <t>vic</t>
+  </si>
+  <si>
+    <t>esto ya lohice en el modulo de usuarios /faltaria modulo de clientes</t>
+  </si>
+  <si>
+    <t>este tambien lo hice igual solo lo verificamos</t>
+  </si>
+  <si>
+    <t>esto lo hacemos en la fase de pruebas</t>
+  </si>
+  <si>
+    <t>rojo pa q te chingue la vista y sepas que es importante jaja</t>
+  </si>
+  <si>
+    <t>este ya lo hice</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,8 +210,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +244,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -228,49 +263,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,590 +630,726 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M26" sqref="A26:M27"/>
+      <selection activeCell="A27" sqref="A27:L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="62.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
       <c r="M3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
       <c r="M5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="N5" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
       <c r="M6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="N7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
       <c r="M10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+    <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
       <c r="M11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
       <c r="M12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+    <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
       <c r="M13" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="N13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
       <c r="M14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="N14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
       <c r="M16" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="N16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="18" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+    <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
       <c r="M19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+    <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="19" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="N20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
       <c r="M21" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    <row r="22" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
       <c r="M22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+    <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
       <c r="M23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
+      <c r="N23" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
       <c r="M24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
       <c r="M25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="10"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
       <c r="M26" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="10"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="10"/>
-      <c r="K27" s="10"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="2" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="N27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="M28" s="15" t="s">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="16" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D29" t="s">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="H29" t="s">
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="M29" s="15"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="16"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="15"/>
+      <c r="B30" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D30" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I30" t="s">
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="M30" s="15"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="16"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M31" s="15"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="16"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="16"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="A33" s="15"/>
+      <c r="B33" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="M33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="16"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="A34" s="15"/>
+      <c r="B34" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="M34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="16"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="15" t="s">
         <v>15</v>
       </c>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="A10:L10"/>
     <mergeCell ref="M28:M35"/>
     <mergeCell ref="A27:L27"/>
     <mergeCell ref="A24:L24"/>
@@ -1184,19 +1365,6 @@
     <mergeCell ref="A11:L11"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A10:L10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
se agregan actividades y detalle de la cotizacion b
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA1580F-EBF8-4669-83EF-4B393BE1FF02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE96781-C4DD-49E5-A250-3480C372E57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
   <si>
     <t>- Agregar precio de menudeo y mayoreo en la información de los productos en venta con una abreviatura que identifique el precio p.e. “Me:” o “Ma:”. Además, cambiar existencias a abreviado “E: ” y si no hay poner “S/E”.</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>este ya lo hice</t>
+  </si>
+  <si>
+    <t>imprimir ticker cuando se realiza un cierre de caja por exceso de efectivo-&gt; Hora y Fecha, Sucursal , Alamcan, Estacion , Nombre Usuario,  Monto , una linea para poner una firma de autorizado</t>
+  </si>
+  <si>
+    <t>imprimir ticker cuando se realiza un cierre de dia-&gt; Hora y Fecha, Sucursal , Alamcan, Estacion , Nombre Usuario,  Monto , una linea para poner una firma de autorizado</t>
   </si>
 </sst>
 </file>
@@ -267,17 +273,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,14 +286,11 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -300,10 +298,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -311,11 +319,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -630,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
-  <dimension ref="A1:N36"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:L27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,36 +648,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -693,80 +699,80 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
       <c r="M4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
       <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
       <c r="M6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
       <c r="M7" t="s">
         <v>33</v>
       </c>
@@ -775,39 +781,39 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
       <c r="M8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
       <c r="M9" t="s">
         <v>32</v>
       </c>
@@ -832,58 +838,58 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
       <c r="M11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
       <c r="M12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
       <c r="M13" t="s">
         <v>32</v>
       </c>
@@ -892,20 +898,20 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
       <c r="M14" t="s">
         <v>35</v>
       </c>
@@ -914,39 +920,39 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="M15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+      <c r="L16" s="8"/>
       <c r="M16" t="s">
         <v>33</v>
       </c>
@@ -955,78 +961,78 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
       <c r="M17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
       <c r="M18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
       <c r="M19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18"/>
-      <c r="M20" s="19" t="s">
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="20"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N20" t="s">
@@ -1034,58 +1040,58 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
-      <c r="K21" s="7"/>
-      <c r="L21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
       <c r="M21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
       <c r="M22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
       <c r="M23" t="s">
         <v>44</v>
       </c>
@@ -1094,249 +1100,301 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
+      <c r="B24" s="16"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
       <c r="M24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-      <c r="L25" s="3"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
       <c r="M25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="17"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+    </row>
+    <row r="27" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="17"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="17"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="2" t="s">
+      <c r="B28" s="17"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="N27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="15"/>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="16" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="D29" s="15"/>
       <c r="E29" s="15"/>
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
-      <c r="H29" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="H29" s="15"/>
       <c r="I29" s="15"/>
       <c r="J29" s="15"/>
       <c r="K29" s="15"/>
       <c r="L29" s="15"/>
-      <c r="M29" s="16"/>
+      <c r="M29" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15" t="s">
+      <c r="A30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15" t="s">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
-      <c r="I30" s="15" t="s">
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="16"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15" t="s">
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15" t="s">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="15"/>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="16"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="15"/>
-      <c r="B33" s="15" t="s">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="15"/>
-      <c r="I33" s="15"/>
-      <c r="J33" s="15"/>
-      <c r="K33" s="15"/>
-      <c r="L33" s="15"/>
-      <c r="M33" s="16"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="15"/>
-      <c r="B34" s="15" t="s">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="15"/>
-      <c r="I34" s="15"/>
-      <c r="J34" s="15"/>
-      <c r="K34" s="15"/>
-      <c r="L34" s="15"/>
-      <c r="M34" s="16"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="15"/>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="16"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
+  <mergeCells count="30">
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M30:M37"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="A27:L27"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="A17:L17"/>
@@ -1350,21 +1408,6 @@
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="A7:L7"/>
     <mergeCell ref="A10:L10"/>
-    <mergeCell ref="M28:M35"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A15:L15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
se modifcan en la app la manera de generar bitacoras
</commit_message>
<xml_diff>
--- a/Analisis/Actividades 4.xlsx
+++ b/Analisis/Actividades 4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BE96781-C4DD-49E5-A250-3480C372E57B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA47EBE5-644B-4638-B546-F8B5E8B71EF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A2A51F05-D945-4770-9981-DCBF9858099F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>- Agregar precio de menudeo y mayoreo en la información de los productos en venta con una abreviatura que identifique el precio p.e. “Me:” o “Ma:”. Además, cambiar existencias a abreviado “E: ” y si no hay poner “S/E”.</t>
   </si>
@@ -231,7 +231,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +256,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -269,10 +275,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -322,6 +327,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C224E-5DA8-45B6-95FA-081980391123}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,131 +656,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
       <c r="M3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
       <c r="M4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="11"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
       <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="3" t="s">
+      <c r="N5" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
       <c r="M7" t="s">
         <v>33</v>
       </c>
@@ -781,115 +789,115 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
       <c r="M8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
       <c r="M9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="21"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
       <c r="M11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
       <c r="M12" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
       <c r="M13" t="s">
         <v>32</v>
       </c>
@@ -898,20 +906,20 @@
       </c>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
       <c r="M14" t="s">
         <v>35</v>
       </c>
@@ -920,39 +928,39 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
       <c r="M16" t="s">
         <v>33</v>
       </c>
@@ -961,78 +969,78 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="M17" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+      <c r="A18" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
       <c r="M18" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
       <c r="M19" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="5" t="s">
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="4" t="s">
         <v>32</v>
       </c>
       <c r="N20" t="s">
@@ -1040,58 +1048,58 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
       <c r="M21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
       <c r="M22" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
       <c r="M23" t="s">
         <v>44</v>
       </c>
@@ -1100,113 +1108,116 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
       <c r="M24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="17"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="17"/>
-      <c r="L25" s="17"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
       <c r="M25" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
-      <c r="F26" s="17"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="22" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-      <c r="M27" t="s">
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="16"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="22" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="2" t="s">
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="6" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="5" t="s">
         <v>33</v>
       </c>
       <c r="N29" t="s">
@@ -1214,167 +1225,167 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-      <c r="M30" s="14" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="s">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4" t="s">
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="14"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" s="13"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4" t="s">
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-      <c r="M32" s="14"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="13"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="14"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="13"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="4"/>
-      <c r="B34" s="4" t="s">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="14"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="13"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="4"/>
-      <c r="B35" s="4" t="s">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="14"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="13"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="14"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="13"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-      <c r="H37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="14"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="13"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="30">

</xml_diff>